<commit_message>
Added sample scripts for processing with and without excel input file.
</commit_message>
<xml_diff>
--- a/examples/input_form.xlsx
+++ b/examples/input_form.xlsx
@@ -5,25 +5,22 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\OneDrive\Work\TaborLab\Code\fc\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="cells" sheetId="1" r:id="rId1"/>
+    <sheet name="beads" sheetId="2" r:id="rId1"/>
+    <sheet name="cells" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>ATC</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>File Path</t>
   </si>
@@ -34,42 +31,56 @@
     <t>Kinase</t>
   </si>
   <si>
-    <t>Sigma</t>
-  </si>
-  <si>
-    <t>beads/data.001</t>
-  </si>
-  <si>
-    <t>cells/data.001</t>
-  </si>
-  <si>
-    <t>cells/data.002</t>
-  </si>
-  <si>
-    <t>cells/data.003</t>
-  </si>
-  <si>
-    <t>cells/data.004</t>
-  </si>
-  <si>
-    <t>cells/data.005</t>
-  </si>
-  <si>
-    <t>Beads Peaks</t>
-  </si>
-  <si>
     <t>Beads File Path</t>
   </si>
   <si>
-    <t>792, 2079, 6588 ,16471, 47497, 137049, 371647</t>
+    <t>FCFiles/data.001</t>
+  </si>
+  <si>
+    <t>FCFiles/data.002</t>
+  </si>
+  <si>
+    <t>FCFiles/data.003</t>
+  </si>
+  <si>
+    <t>FCFiles/data.004</t>
+  </si>
+  <si>
+    <t>FCFiles/data.005</t>
+  </si>
+  <si>
+    <t>MEFL</t>
+  </si>
+  <si>
+    <t>FCFiles/data.006</t>
+  </si>
+  <si>
+    <t>Clustering Method</t>
+  </si>
+  <si>
+    <t>gmm</t>
+  </si>
+  <si>
+    <t>aTc</t>
+  </si>
+  <si>
+    <t>None, 792, 2079, 6588, 16471, 47497, 137049, 271647</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -97,13 +108,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -410,161 +429,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>0.3</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="E2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
         <v>0.2</v>
       </c>
-      <c r="E2" s="1">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="D4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="G3" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="1">
+      <c r="C6" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="2">
         <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E8" s="1">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>